<commit_message>
Added relevance_check in the helpers.py file. Halts scraping once articles become irrelevant
</commit_message>
<xml_diff>
--- a/scraped_articles.xlsx
+++ b/scraped_articles.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -413,14 +425,162 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Synopsis</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Patience pays off in quantum computing</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/63cf560a-69f3-42c2-82c3-7e8d97282716</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quantum computing is struggling to reach its silicon moment</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/bfe5fff4-3d78-4bea-9e31-da8ca1f77151</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Quantum computing is overshadowed by rapid advances in AI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/e3e2b721-9971-47b1-aa86-f210804ebc3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Letter: Quantum computing does the hard stuff AI alone can’t crack</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/bc1298fd-868c-4c21-b9c1-81716b583c7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Scientific breakthrough gives new hope to building quantum computers</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/f1d26918-67c5-4b11-b47b-4904606a002f</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Microsoft claims quantum breakthrough after 20-year pursuit of elusive particle</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/a60f44f5-81ca-4e66-8193-64c956b09820</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The mysterious promise of the quantum future</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/7ce2f04a-f8e2-4e3d-8602-776647c520c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Quantum computing breakthroughs draw investment back to sector</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/d0b486ab-ed6c-46f0-b7b6-66cc60780efe</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>